<commit_message>
feat: implement feature extraction for categories B, C and D
</commit_message>
<xml_diff>
--- a/features_category_b.xlsx
+++ b/features_category_b.xlsx
@@ -467,19 +467,19 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.01461682877891991</v>
+        <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.6536770345289048</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0.01460360101157396</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>2.90410644732146</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>-5.450237561760327</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -487,19 +487,19 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.1728643399999989</v>
+        <v>0.158198511282029</v>
       </c>
       <c r="B3" t="n">
-        <v>1.726891795775603</v>
+        <v>2.382964774536509</v>
       </c>
       <c r="C3" t="n">
-        <v>0.05345242601967008</v>
+        <v>0.05411120097525475</v>
       </c>
       <c r="D3" t="n">
-        <v>232.5090162211441</v>
+        <v>247.8342241219283</v>
       </c>
       <c r="E3" t="n">
-        <v>-341.2981389385268</v>
+        <v>-328.1946692603154</v>
       </c>
       <c r="F3" t="n">
         <v>1</v>
@@ -507,19 +507,19 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.1686058266666655</v>
+        <v>0.1540195103665217</v>
       </c>
       <c r="B4" t="n">
-        <v>1.106598544986156</v>
+        <v>1.788466067858054</v>
       </c>
       <c r="C4" t="n">
-        <v>0.05902422017440354</v>
+        <v>0.0586987627156471</v>
       </c>
       <c r="D4" t="n">
-        <v>284.8276825796112</v>
+        <v>303.4561756544852</v>
       </c>
       <c r="E4" t="n">
-        <v>-221.5776036302574</v>
+        <v>-208.5430616732992</v>
       </c>
       <c r="F4" t="n">
         <v>2</v>
@@ -527,19 +527,19 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.1524477599999987</v>
+        <v>0.1376840416828386</v>
       </c>
       <c r="B5" t="n">
-        <v>0.5709679500941993</v>
+        <v>1.205309520067421</v>
       </c>
       <c r="C5" t="n">
-        <v>0.05109702746579042</v>
+        <v>0.05003394674851547</v>
       </c>
       <c r="D5" t="n">
-        <v>280.0321931813189</v>
+        <v>293.6285991707177</v>
       </c>
       <c r="E5" t="n">
-        <v>-266.9804431420322</v>
+        <v>-257.60970680964</v>
       </c>
       <c r="F5" t="n">
         <v>3</v>
@@ -547,19 +547,19 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.1166450242424227</v>
+        <v>0.1019788141093302</v>
       </c>
       <c r="B6" t="n">
-        <v>0.8326149783915793</v>
+        <v>1.504276112067938</v>
       </c>
       <c r="C6" t="n">
-        <v>0.03409674077543669</v>
+        <v>0.03327306634794119</v>
       </c>
       <c r="D6" t="n">
-        <v>340.8115996962164</v>
+        <v>340.048837864487</v>
       </c>
       <c r="E6" t="n">
-        <v>-308.2994365764368</v>
+        <v>-305.2886354542786</v>
       </c>
       <c r="F6" t="n">
         <v>4</v>
@@ -567,19 +567,19 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.1310955818181801</v>
+        <v>0.1167150697089643</v>
       </c>
       <c r="B7" t="n">
-        <v>1.045055280971326</v>
+        <v>1.685242637903506</v>
       </c>
       <c r="C7" t="n">
-        <v>0.03513250032469948</v>
+        <v>0.03231202834206442</v>
       </c>
       <c r="D7" t="n">
-        <v>340.3935972893077</v>
+        <v>338.8017652129342</v>
       </c>
       <c r="E7" t="n">
-        <v>-299.8507895223406</v>
+        <v>-300.9313775146296</v>
       </c>
       <c r="F7" t="n">
         <v>5</v>
@@ -587,19 +587,19 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.1154471466666654</v>
+        <v>0.1009261513800769</v>
       </c>
       <c r="B8" t="n">
-        <v>0.5764486838405821</v>
+        <v>1.225863637484949</v>
       </c>
       <c r="C8" t="n">
-        <v>0.03401543262826116</v>
+        <v>0.03162228579006612</v>
       </c>
       <c r="D8" t="n">
-        <v>397.9325953967983</v>
+        <v>396.8258629731951</v>
       </c>
       <c r="E8" t="n">
-        <v>-259.4258982479697</v>
+        <v>-253.9037553476354</v>
       </c>
       <c r="F8" t="n">
         <v>6</v>
@@ -607,19 +607,19 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.0755528266666657</v>
+        <v>0.06094166116993887</v>
       </c>
       <c r="B9" t="n">
-        <v>0.1054074822819476</v>
+        <v>0.7625901528269406</v>
       </c>
       <c r="C9" t="n">
-        <v>0.02351459052264597</v>
+        <v>0.01849781433443191</v>
       </c>
       <c r="D9" t="n">
-        <v>192.1938709167994</v>
+        <v>192.9238904066669</v>
       </c>
       <c r="E9" t="n">
-        <v>-176.803078937943</v>
+        <v>-177.8628334406862</v>
       </c>
       <c r="F9" t="n">
         <v>7</v>
@@ -627,19 +627,19 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.08555979666666559</v>
+        <v>0.07118947121057537</v>
       </c>
       <c r="B10" t="n">
-        <v>0.4343685029898836</v>
+        <v>1.119460267558798</v>
       </c>
       <c r="C10" t="n">
-        <v>0.02585716704468571</v>
+        <v>0.02337542951264013</v>
       </c>
       <c r="D10" t="n">
-        <v>192.3915993930445</v>
+        <v>192.6881573065673</v>
       </c>
       <c r="E10" t="n">
-        <v>-186.142059491945</v>
+        <v>-185.8109313328811</v>
       </c>
       <c r="F10" t="n">
         <v>8</v>
@@ -647,19 +647,19 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.06898184333333222</v>
+        <v>0.0541078498096448</v>
       </c>
       <c r="B11" t="n">
-        <v>0.1067754478097013</v>
+        <v>0.7588137205112726</v>
       </c>
       <c r="C11" t="n">
-        <v>0.02190872016322986</v>
+        <v>0.01852106772350293</v>
       </c>
       <c r="D11" t="n">
-        <v>197.2585413971364</v>
+        <v>197.0010493325451</v>
       </c>
       <c r="E11" t="n">
-        <v>-192.34991899551</v>
+        <v>-192.5617075595327</v>
       </c>
       <c r="F11" t="n">
         <v>9</v>
@@ -667,19 +667,19 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.05163072666666586</v>
+        <v>0.03714639929402445</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.411430301099152</v>
+        <v>0.2436152250794927</v>
       </c>
       <c r="C12" t="n">
-        <v>0.02158858989741641</v>
+        <v>0.01563910710119206</v>
       </c>
       <c r="D12" t="n">
-        <v>91.81050562984844</v>
+        <v>93.62070615841097</v>
       </c>
       <c r="E12" t="n">
-        <v>-128.9796578485333</v>
+        <v>-126.5700158953849</v>
       </c>
       <c r="F12" t="n">
         <v>10</v>
@@ -687,19 +687,19 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.04136679666666598</v>
+        <v>0.02670730936268782</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.1045325132266157</v>
+        <v>0.5478846551529415</v>
       </c>
       <c r="C13" t="n">
-        <v>0.01477798672358223</v>
+        <v>0.01179336757600432</v>
       </c>
       <c r="D13" t="n">
-        <v>104.408713663341</v>
+        <v>104.6479971095391</v>
       </c>
       <c r="E13" t="n">
-        <v>-115.2323676483018</v>
+        <v>-113.8645512141335</v>
       </c>
       <c r="F13" t="n">
         <v>11</v>
@@ -707,19 +707,19 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.05533729666666595</v>
+        <v>0.0408770819726052</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.4143575405123756</v>
+        <v>0.2522657329159978</v>
       </c>
       <c r="C14" t="n">
-        <v>0.02240326922942375</v>
+        <v>0.01478029039727919</v>
       </c>
       <c r="D14" t="n">
-        <v>97.00017227548516</v>
+        <v>97.73063300077291</v>
       </c>
       <c r="E14" t="n">
-        <v>-120.6684954716332</v>
+        <v>-118.9361617004882</v>
       </c>
       <c r="F14" t="n">
         <v>12</v>
@@ -727,19 +727,19 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.03083268541666636</v>
+        <v>0.01637990724578956</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.3530350083615315</v>
+        <v>0.3090364102667344</v>
       </c>
       <c r="C15" t="n">
-        <v>0.01627834077565099</v>
+        <v>0.005688285407817011</v>
       </c>
       <c r="D15" t="n">
-        <v>67.85116839020948</v>
+        <v>67.7750465728467</v>
       </c>
       <c r="E15" t="n">
-        <v>-82.37334929515536</v>
+        <v>-80.43421957432557</v>
       </c>
       <c r="F15" t="n">
         <v>13</v>
@@ -747,19 +747,19 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.02983729999999946</v>
+        <v>0.01514138919410355</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.2395837204645644</v>
+        <v>0.4120035099296989</v>
       </c>
       <c r="C16" t="n">
-        <v>0.01230040816995616</v>
+        <v>0.009063658100976027</v>
       </c>
       <c r="D16" t="n">
-        <v>72.42107978297658</v>
+        <v>73.00548254706821</v>
       </c>
       <c r="E16" t="n">
-        <v>-74.35767362446802</v>
+        <v>-73.37087307661103</v>
       </c>
       <c r="F16" t="n">
         <v>14</v>
@@ -767,19 +767,19 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0.03187929999999949</v>
+        <v>0.01695514102691537</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.2900484156769752</v>
+        <v>0.3271829186070354</v>
       </c>
       <c r="C17" t="n">
-        <v>0.01450449659839718</v>
+        <v>0.005380600201584886</v>
       </c>
       <c r="D17" t="n">
-        <v>61.94034942630909</v>
+        <v>62.20673974235961</v>
       </c>
       <c r="E17" t="n">
-        <v>-81.33530838608252</v>
+        <v>-79.38237905458644</v>
       </c>
       <c r="F17" t="n">
         <v>15</v>
@@ -787,19 +787,19 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0.02738696666666629</v>
+        <v>0.01277602165241459</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.4952661885593346</v>
+        <v>0.1632611229311623</v>
       </c>
       <c r="C18" t="n">
-        <v>0.01410683746600191</v>
+        <v>0.006320965955682019</v>
       </c>
       <c r="D18" t="n">
-        <v>21.88413086905823</v>
+        <v>27.15632824073893</v>
       </c>
       <c r="E18" t="n">
-        <v>-73.6461392413985</v>
+        <v>-50.78388276646678</v>
       </c>
       <c r="F18" t="n">
         <v>16</v>
@@ -807,19 +807,19 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0.02356666666666625</v>
+        <v>0.009184853667081782</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.4831209571760535</v>
+        <v>0.1876403846026099</v>
       </c>
       <c r="C19" t="n">
-        <v>0.01344244939790621</v>
+        <v>0.005946669553404348</v>
       </c>
       <c r="D19" t="n">
-        <v>29.93576416041295</v>
+        <v>31.26249992272761</v>
       </c>
       <c r="E19" t="n">
-        <v>-66.30320178915427</v>
+        <v>-67.37116608050415</v>
       </c>
       <c r="F19" t="n">
         <v>17</v>
@@ -827,19 +827,19 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.0176335428571426</v>
+        <v>0.002866464322252697</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.4193371263871641</v>
+        <v>0.2435478807864958</v>
       </c>
       <c r="C20" t="n">
-        <v>0.01066363981611673</v>
+        <v>0.008378269355337786</v>
       </c>
       <c r="D20" t="n">
-        <v>31.99562501018345</v>
+        <v>34.34349841099724</v>
       </c>
       <c r="E20" t="n">
-        <v>-76.24182983192378</v>
+        <v>-72.29254313702833</v>
       </c>
       <c r="F20" t="n">
         <v>18</v>
@@ -847,19 +847,19 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.01688125520833304</v>
+        <v>0.002078510743094199</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.4759898255524046</v>
+        <v>0.1845282344935664</v>
       </c>
       <c r="C21" t="n">
-        <v>0.01193641439824343</v>
+        <v>0.005325596082023524</v>
       </c>
       <c r="D21" t="n">
-        <v>28.25464481318303</v>
+        <v>35.54178086282234</v>
       </c>
       <c r="E21" t="n">
-        <v>-84.48462977081785</v>
+        <v>-70.26433410178562</v>
       </c>
       <c r="F21" t="n">
         <v>19</v>
@@ -867,19 +867,19 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0.0256956999999996</v>
+        <v>0.01097339483756912</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.516632783353136</v>
+        <v>0.1262704788765468</v>
       </c>
       <c r="C22" t="n">
-        <v>0.0143637551531884</v>
+        <v>0.004769659520192954</v>
       </c>
       <c r="D22" t="n">
-        <v>38.00209543046215</v>
+        <v>43.28600926053447</v>
       </c>
       <c r="E22" t="n">
-        <v>-61.93016930583573</v>
+        <v>-41.65370072769352</v>
       </c>
       <c r="F22" t="n">
         <v>20</v>
@@ -887,19 +887,19 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0.02085103854166638</v>
+        <v>0.006234698565036533</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.4791163098488145</v>
+        <v>0.1822255452505377</v>
       </c>
       <c r="C23" t="n">
-        <v>0.01254157844963881</v>
+        <v>0.006497059408533399</v>
       </c>
       <c r="D23" t="n">
-        <v>21.1960434028457</v>
+        <v>27.67473969566274</v>
       </c>
       <c r="E23" t="n">
-        <v>-72.19888026138942</v>
+        <v>-57.40356582818455</v>
       </c>
       <c r="F23" t="n">
         <v>21</v>
@@ -907,19 +907,19 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0.0198869323601969</v>
+        <v>0.00513491467248337</v>
       </c>
       <c r="B24" t="n">
-        <v>-0.6493123890965078</v>
+        <v>0.00588135787470902</v>
       </c>
       <c r="C24" t="n">
-        <v>0.01457858597115233</v>
+        <v>0.004168230232110934</v>
       </c>
       <c r="D24" t="n">
-        <v>38.06348417639627</v>
+        <v>42.91778683065272</v>
       </c>
       <c r="E24" t="n">
-        <v>-56.92832554438967</v>
+        <v>-40.41788011606975</v>
       </c>
       <c r="F24" t="n">
         <v>22</v>
@@ -927,19 +927,19 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0.0201829787709797</v>
+        <v>0.005376217746727448</v>
       </c>
       <c r="B25" t="n">
-        <v>-0.6677052844668819</v>
+        <v>-0.02325644003000819</v>
       </c>
       <c r="C25" t="n">
-        <v>0.01529077329480307</v>
+        <v>0.003758026797506845</v>
       </c>
       <c r="D25" t="n">
-        <v>29.37582716036992</v>
+        <v>35.20149788051975</v>
       </c>
       <c r="E25" t="n">
-        <v>-59.75109517053833</v>
+        <v>-46.65545164026287</v>
       </c>
       <c r="F25" t="n">
         <v>23</v>
@@ -947,19 +947,19 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0.01942165245889042</v>
+        <v>0.00483635662983685</v>
       </c>
       <c r="B26" t="n">
-        <v>-0.6041265854581093</v>
+        <v>0.05741663671836112</v>
       </c>
       <c r="C26" t="n">
-        <v>0.01393560204946034</v>
+        <v>0.003730438096506507</v>
       </c>
       <c r="D26" t="n">
-        <v>46.48894368597867</v>
+        <v>48.08190431054824</v>
       </c>
       <c r="E26" t="n">
-        <v>-67.5379172464626</v>
+        <v>-64.59116634311304</v>
       </c>
       <c r="F26" t="n">
         <v>24</v>
@@ -967,19 +967,19 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>0.01717669349123039</v>
+        <v>0.0026746514566514</v>
       </c>
       <c r="B27" t="n">
-        <v>-0.6506999808115228</v>
+        <v>0.01584425828584345</v>
       </c>
       <c r="C27" t="n">
-        <v>0.01486336823295298</v>
+        <v>0.002063345441072744</v>
       </c>
       <c r="D27" t="n">
-        <v>33.33084147069216</v>
+        <v>39.84994971997929</v>
       </c>
       <c r="E27" t="n">
-        <v>-68.31909724871178</v>
+        <v>-56.53078962697166</v>
       </c>
       <c r="F27" t="n">
         <v>25</v>
@@ -987,19 +987,19 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>0.02122841387036161</v>
+        <v>0.006714176797792768</v>
       </c>
       <c r="B28" t="n">
-        <v>-0.6803653909792891</v>
+        <v>-0.03158908954096089</v>
       </c>
       <c r="C28" t="n">
-        <v>0.01608332701901607</v>
+        <v>0.004751901111793445</v>
       </c>
       <c r="D28" t="n">
-        <v>37.76875511559213</v>
+        <v>39.16005634655902</v>
       </c>
       <c r="E28" t="n">
-        <v>-51.75771851419073</v>
+        <v>-51.99881467912345</v>
       </c>
       <c r="F28" t="n">
         <v>26</v>
@@ -1007,19 +1007,19 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>0.01304621389018141</v>
+        <v>-0.001693836225436336</v>
       </c>
       <c r="B29" t="n">
-        <v>-0.4604286306729339</v>
+        <v>0.2072997783691784</v>
       </c>
       <c r="C29" t="n">
-        <v>0.01086760150764513</v>
+        <v>0.005098871097328627</v>
       </c>
       <c r="D29" t="n">
-        <v>36.81280712484584</v>
+        <v>41.76056848758277</v>
       </c>
       <c r="E29" t="n">
-        <v>-55.48258067246545</v>
+        <v>-37.99410850835997</v>
       </c>
       <c r="F29" t="n">
         <v>27</v>
@@ -1027,19 +1027,19 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0.0171354159736838</v>
+        <v>0.002330665727222756</v>
       </c>
       <c r="B30" t="n">
-        <v>-0.557945038109792</v>
+        <v>0.08029727403436233</v>
       </c>
       <c r="C30" t="n">
-        <v>0.01327944039906333</v>
+        <v>0.003238637763507987</v>
       </c>
       <c r="D30" t="n">
-        <v>32.62328107762917</v>
+        <v>38.37018805138749</v>
       </c>
       <c r="E30" t="n">
-        <v>-65.38925204724993</v>
+        <v>-50.28915177815563</v>
       </c>
       <c r="F30" t="n">
         <v>28</v>
@@ -1047,19 +1047,19 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>0.01669786562914701</v>
+        <v>0.001851609066906718</v>
       </c>
       <c r="B31" t="n">
-        <v>-0.5791854679963012</v>
+        <v>0.06012627387253142</v>
       </c>
       <c r="C31" t="n">
-        <v>0.01377611248523513</v>
+        <v>0.002653532385341967</v>
       </c>
       <c r="D31" t="n">
-        <v>30.1270817298185</v>
+        <v>32.22939598880857</v>
       </c>
       <c r="E31" t="n">
-        <v>-70.00280588147028</v>
+        <v>-66.33103358886862</v>
       </c>
       <c r="F31" t="n">
         <v>29</v>
@@ -1067,19 +1067,19 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>0.02460342249999979</v>
+        <v>0.0100494872671646</v>
       </c>
       <c r="B32" t="n">
-        <v>-1.00242956574095</v>
+        <v>-0.3598738674937444</v>
       </c>
       <c r="C32" t="n">
-        <v>0.02196530719355606</v>
+        <v>0.006856646187861419</v>
       </c>
       <c r="D32" t="n">
-        <v>8.958492269745213</v>
+        <v>11.01814695122591</v>
       </c>
       <c r="E32" t="n">
-        <v>-12.1072120678675</v>
+        <v>-9.608064070489965</v>
       </c>
       <c r="F32" t="n">
         <v>30</v>
@@ -1087,19 +1087,19 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>0.01531722854212956</v>
+        <v>0.0007339728299216452</v>
       </c>
       <c r="B33" t="n">
-        <v>-0.7023149468219592</v>
+        <v>-0.04715314444366168</v>
       </c>
       <c r="C33" t="n">
-        <v>0.01645038932621356</v>
+        <v>0.001510929242360452</v>
       </c>
       <c r="D33" t="n">
-        <v>17.33980085159854</v>
+        <v>19.78744087512309</v>
       </c>
       <c r="E33" t="n">
-        <v>-92.01874341558198</v>
+        <v>-59.21353538232588</v>
       </c>
       <c r="F33" t="n">
         <v>31</v>
@@ -1107,19 +1107,19 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>0.02005938349849735</v>
+        <v>0.00565511710181539</v>
       </c>
       <c r="B34" t="n">
-        <v>-0.8371256729959539</v>
+        <v>-0.1822266930381763</v>
       </c>
       <c r="C34" t="n">
-        <v>0.01795984244250423</v>
+        <v>0.004259163515995619</v>
       </c>
       <c r="D34" t="n">
-        <v>19.53146198129168</v>
+        <v>20.9308915086084</v>
       </c>
       <c r="E34" t="n">
-        <v>-86.86632210679339</v>
+        <v>-50.3774663521443</v>
       </c>
       <c r="F34" t="n">
         <v>32</v>
@@ -1127,19 +1127,19 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>0.01970191438883411</v>
+        <v>0.005019019614673753</v>
       </c>
       <c r="B35" t="n">
-        <v>-0.7928128300649631</v>
+        <v>-0.1619196163743815</v>
       </c>
       <c r="C35" t="n">
-        <v>0.01857757543702953</v>
+        <v>0.004201990327278174</v>
       </c>
       <c r="D35" t="n">
-        <v>13.67992466406772</v>
+        <v>19.57587411217437</v>
       </c>
       <c r="E35" t="n">
-        <v>-108.7760421171382</v>
+        <v>-49.4390421254724</v>
       </c>
       <c r="F35" t="n">
         <v>33</v>
@@ -1147,19 +1147,19 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>0.01616103368388381</v>
+        <v>0.001585721261110376</v>
       </c>
       <c r="B36" t="n">
-        <v>-0.734478853182179</v>
+        <v>-0.08420676243206225</v>
       </c>
       <c r="C36" t="n">
-        <v>0.01680391572955407</v>
+        <v>0.001781603747779381</v>
       </c>
       <c r="D36" t="n">
-        <v>19.44638498139446</v>
+        <v>20.80094986944983</v>
       </c>
       <c r="E36" t="n">
-        <v>-82.5016456698483</v>
+        <v>-50.18766739303585</v>
       </c>
       <c r="F36" t="n">
         <v>34</v>
@@ -1167,19 +1167,19 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>0.01818225848422167</v>
+        <v>0.003638466906014801</v>
       </c>
       <c r="B37" t="n">
-        <v>-0.7876842709308626</v>
+        <v>-0.1331171612016337</v>
       </c>
       <c r="C37" t="n">
-        <v>0.0171391945227682</v>
+        <v>0.002538966893398722</v>
       </c>
       <c r="D37" t="n">
-        <v>11.37741414608984</v>
+        <v>12.98525938162125</v>
       </c>
       <c r="E37" t="n">
-        <v>-90.38536625301616</v>
+        <v>-63.76945084478938</v>
       </c>
       <c r="F37" t="n">
         <v>35</v>
@@ -1187,19 +1187,19 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>0.01969223741332427</v>
+        <v>0.004996495700326854</v>
       </c>
       <c r="B38" t="n">
-        <v>-0.8308961020123463</v>
+        <v>-0.1896409366880591</v>
       </c>
       <c r="C38" t="n">
-        <v>0.01939952079340379</v>
+        <v>0.00425573512797767</v>
       </c>
       <c r="D38" t="n">
-        <v>13.41435035713817</v>
+        <v>16.0994107644036</v>
       </c>
       <c r="E38" t="n">
-        <v>-101.2166942433644</v>
+        <v>-73.56742789005463</v>
       </c>
       <c r="F38" t="n">
         <v>36</v>
@@ -1207,19 +1207,19 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>0.02196707833790037</v>
+        <v>0.007419953615086644</v>
       </c>
       <c r="B39" t="n">
-        <v>-0.8473047673472126</v>
+        <v>-0.1921566973228025</v>
       </c>
       <c r="C39" t="n">
-        <v>0.01817307655378766</v>
+        <v>0.004808294806688117</v>
       </c>
       <c r="D39" t="n">
-        <v>16.28047606733938</v>
+        <v>18.08096162301872</v>
       </c>
       <c r="E39" t="n">
-        <v>-82.83675410526831</v>
+        <v>-46.98239848817071</v>
       </c>
       <c r="F39" t="n">
         <v>37</v>
@@ -1227,19 +1227,19 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>0.02534582564787492</v>
+        <v>0.01100494228349626</v>
       </c>
       <c r="B40" t="n">
-        <v>-1.087081346340353</v>
+        <v>-0.4391384069867468</v>
       </c>
       <c r="C40" t="n">
-        <v>0.0242421500529274</v>
+        <v>0.007817119392250431</v>
       </c>
       <c r="D40" t="n">
-        <v>13.65391634351252</v>
+        <v>12.56635015022701</v>
       </c>
       <c r="E40" t="n">
-        <v>-7.120863890885294</v>
+        <v>-9.350520304598183</v>
       </c>
       <c r="F40" t="n">
         <v>38</v>
@@ -1247,19 +1247,19 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>0.01331892569291484</v>
+        <v>-0.001403690472340024</v>
       </c>
       <c r="B41" t="n">
-        <v>-0.5294083889143649</v>
+        <v>0.1212159762492618</v>
       </c>
       <c r="C41" t="n">
-        <v>0.01218165047656732</v>
+        <v>0.002633551022753115</v>
       </c>
       <c r="D41" t="n">
-        <v>18.04556296199106</v>
+        <v>19.24442053694606</v>
       </c>
       <c r="E41" t="n">
-        <v>-72.9745672578326</v>
+        <v>-49.12251450380327</v>
       </c>
       <c r="F41" t="n">
         <v>39</v>
@@ -1267,19 +1267,19 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>0.01866133842757729</v>
+        <v>0.003998759063008198</v>
       </c>
       <c r="B42" t="n">
-        <v>-0.7226529194067504</v>
+        <v>-0.07155415964064167</v>
       </c>
       <c r="C42" t="n">
-        <v>0.01705057858899306</v>
+        <v>0.003232474042622202</v>
       </c>
       <c r="D42" t="n">
-        <v>18.010380305741</v>
+        <v>19.59803963002415</v>
       </c>
       <c r="E42" t="n">
-        <v>-88.34238076227761</v>
+        <v>-52.0593832450757</v>
       </c>
       <c r="F42" t="n">
         <v>40</v>

</xml_diff>

<commit_message>
(feat): add more electrochemical features
</commit_message>
<xml_diff>
--- a/features_category_b.xlsx
+++ b/features_category_b.xlsx
@@ -467,19 +467,19 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
+        <v>0.01461682877891991</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>-0.6536770345289049</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>0.01460360101157396</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>2.90410644732146</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>-5.450237561760328</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -487,19 +487,19 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.158198511282029</v>
+        <v>0.1728643399999989</v>
       </c>
       <c r="B3" t="n">
-        <v>2.382964774536509</v>
+        <v>1.726891795775603</v>
       </c>
       <c r="C3" t="n">
-        <v>0.05411120097525475</v>
+        <v>0.05345242601967006</v>
       </c>
       <c r="D3" t="n">
-        <v>247.8342241219283</v>
+        <v>232.5090162211441</v>
       </c>
       <c r="E3" t="n">
-        <v>-328.1946692603154</v>
+        <v>-341.2981389385268</v>
       </c>
       <c r="F3" t="n">
         <v>1</v>
@@ -507,19 +507,19 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.1540195103665217</v>
+        <v>0.1686058266666655</v>
       </c>
       <c r="B4" t="n">
-        <v>1.788466067858054</v>
+        <v>1.106598544986156</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0586987627156471</v>
+        <v>0.05902422017440354</v>
       </c>
       <c r="D4" t="n">
-        <v>303.4561756544852</v>
+        <v>284.8276825796112</v>
       </c>
       <c r="E4" t="n">
-        <v>-208.5430616732992</v>
+        <v>-221.5776036302574</v>
       </c>
       <c r="F4" t="n">
         <v>2</v>
@@ -527,19 +527,19 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.1376840416828386</v>
+        <v>0.1524477599999987</v>
       </c>
       <c r="B5" t="n">
-        <v>1.205309520067421</v>
+        <v>0.5709679500941993</v>
       </c>
       <c r="C5" t="n">
-        <v>0.05003394674851547</v>
+        <v>0.05109702746579042</v>
       </c>
       <c r="D5" t="n">
-        <v>293.6285991707177</v>
+        <v>280.0321931813189</v>
       </c>
       <c r="E5" t="n">
-        <v>-257.60970680964</v>
+        <v>-266.9804431420322</v>
       </c>
       <c r="F5" t="n">
         <v>3</v>
@@ -547,19 +547,19 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.1019788141093302</v>
+        <v>0.1166450242424227</v>
       </c>
       <c r="B6" t="n">
-        <v>1.504276112067938</v>
+        <v>0.8326149783915795</v>
       </c>
       <c r="C6" t="n">
-        <v>0.03327306634794119</v>
+        <v>0.03409674077543669</v>
       </c>
       <c r="D6" t="n">
-        <v>340.048837864487</v>
+        <v>340.8115996962164</v>
       </c>
       <c r="E6" t="n">
-        <v>-305.2886354542786</v>
+        <v>-308.2994365764367</v>
       </c>
       <c r="F6" t="n">
         <v>4</v>
@@ -567,19 +567,19 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.1167150697089643</v>
+        <v>0.1310955818181801</v>
       </c>
       <c r="B7" t="n">
-        <v>1.685242637903506</v>
+        <v>1.045055280971326</v>
       </c>
       <c r="C7" t="n">
-        <v>0.03231202834206442</v>
+        <v>0.03513250032469947</v>
       </c>
       <c r="D7" t="n">
-        <v>338.8017652129342</v>
+        <v>340.3935972893077</v>
       </c>
       <c r="E7" t="n">
-        <v>-300.9313775146296</v>
+        <v>-299.8507895223406</v>
       </c>
       <c r="F7" t="n">
         <v>5</v>
@@ -587,19 +587,19 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.1009261513800769</v>
+        <v>0.1154471466666654</v>
       </c>
       <c r="B8" t="n">
-        <v>1.225863637484949</v>
+        <v>0.5764486838405825</v>
       </c>
       <c r="C8" t="n">
-        <v>0.03162228579006612</v>
+        <v>0.03401543262826115</v>
       </c>
       <c r="D8" t="n">
-        <v>396.8258629731951</v>
+        <v>397.9325953967981</v>
       </c>
       <c r="E8" t="n">
-        <v>-253.9037553476354</v>
+        <v>-259.4258982479697</v>
       </c>
       <c r="F8" t="n">
         <v>6</v>
@@ -607,19 +607,19 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.06094166116993887</v>
+        <v>0.0755528266666657</v>
       </c>
       <c r="B9" t="n">
-        <v>0.7625901528269406</v>
+        <v>0.1054074822819475</v>
       </c>
       <c r="C9" t="n">
-        <v>0.01849781433443191</v>
+        <v>0.02351459052264597</v>
       </c>
       <c r="D9" t="n">
-        <v>192.9238904066669</v>
+        <v>192.1938709167994</v>
       </c>
       <c r="E9" t="n">
-        <v>-177.8628334406862</v>
+        <v>-176.803078937943</v>
       </c>
       <c r="F9" t="n">
         <v>7</v>
@@ -627,19 +627,19 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.07118947121057537</v>
+        <v>0.08555979666666559</v>
       </c>
       <c r="B10" t="n">
-        <v>1.119460267558798</v>
+        <v>0.4343685029898836</v>
       </c>
       <c r="C10" t="n">
-        <v>0.02337542951264013</v>
+        <v>0.02585716704468571</v>
       </c>
       <c r="D10" t="n">
-        <v>192.6881573065673</v>
+        <v>192.3915993930445</v>
       </c>
       <c r="E10" t="n">
-        <v>-185.8109313328811</v>
+        <v>-186.142059491945</v>
       </c>
       <c r="F10" t="n">
         <v>8</v>
@@ -647,19 +647,19 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.0541078498096448</v>
+        <v>0.06898184333333222</v>
       </c>
       <c r="B11" t="n">
-        <v>0.7588137205112726</v>
+        <v>0.1067754478097014</v>
       </c>
       <c r="C11" t="n">
-        <v>0.01852106772350293</v>
+        <v>0.02190872016322986</v>
       </c>
       <c r="D11" t="n">
-        <v>197.0010493325451</v>
+        <v>197.2585413971364</v>
       </c>
       <c r="E11" t="n">
-        <v>-192.5617075595327</v>
+        <v>-192.34991899551</v>
       </c>
       <c r="F11" t="n">
         <v>9</v>
@@ -667,19 +667,19 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.03714639929402445</v>
+        <v>0.05163072666666586</v>
       </c>
       <c r="B12" t="n">
-        <v>0.2436152250794927</v>
+        <v>-0.411430301099152</v>
       </c>
       <c r="C12" t="n">
-        <v>0.01563910710119206</v>
+        <v>0.0215885898974164</v>
       </c>
       <c r="D12" t="n">
-        <v>93.62070615841097</v>
+        <v>91.81050562984844</v>
       </c>
       <c r="E12" t="n">
-        <v>-126.5700158953849</v>
+        <v>-128.9796578485333</v>
       </c>
       <c r="F12" t="n">
         <v>10</v>
@@ -687,19 +687,19 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.02670730936268782</v>
+        <v>0.04136679666666598</v>
       </c>
       <c r="B13" t="n">
-        <v>0.5478846551529415</v>
+        <v>-0.1045325132266157</v>
       </c>
       <c r="C13" t="n">
-        <v>0.01179336757600432</v>
+        <v>0.01477798672358223</v>
       </c>
       <c r="D13" t="n">
-        <v>104.6479971095391</v>
+        <v>104.408713663341</v>
       </c>
       <c r="E13" t="n">
-        <v>-113.8645512141335</v>
+        <v>-115.2323676483018</v>
       </c>
       <c r="F13" t="n">
         <v>11</v>
@@ -707,19 +707,19 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.0408770819726052</v>
+        <v>0.05533729666666595</v>
       </c>
       <c r="B14" t="n">
-        <v>0.2522657329159978</v>
+        <v>-0.4143575405123757</v>
       </c>
       <c r="C14" t="n">
-        <v>0.01478029039727919</v>
+        <v>0.02240326922942375</v>
       </c>
       <c r="D14" t="n">
-        <v>97.73063300077291</v>
+        <v>97.00017227548516</v>
       </c>
       <c r="E14" t="n">
-        <v>-118.9361617004882</v>
+        <v>-120.6684954716332</v>
       </c>
       <c r="F14" t="n">
         <v>12</v>
@@ -727,19 +727,19 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.01637990724578956</v>
+        <v>0.03083268541666636</v>
       </c>
       <c r="B15" t="n">
-        <v>0.3090364102667344</v>
+        <v>-0.3530350083615316</v>
       </c>
       <c r="C15" t="n">
-        <v>0.005688285407817011</v>
+        <v>0.01627834077565098</v>
       </c>
       <c r="D15" t="n">
-        <v>67.7750465728467</v>
+        <v>67.85116839020948</v>
       </c>
       <c r="E15" t="n">
-        <v>-80.43421957432557</v>
+        <v>-82.37334929515534</v>
       </c>
       <c r="F15" t="n">
         <v>13</v>
@@ -747,19 +747,19 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.01514138919410355</v>
+        <v>0.02983729999999946</v>
       </c>
       <c r="B16" t="n">
-        <v>0.4120035099296989</v>
+        <v>-0.2395837204645644</v>
       </c>
       <c r="C16" t="n">
-        <v>0.009063658100976027</v>
+        <v>0.01230040816995616</v>
       </c>
       <c r="D16" t="n">
-        <v>73.00548254706821</v>
+        <v>72.42107978297658</v>
       </c>
       <c r="E16" t="n">
-        <v>-73.37087307661103</v>
+        <v>-74.35767362446802</v>
       </c>
       <c r="F16" t="n">
         <v>14</v>
@@ -767,19 +767,19 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0.01695514102691537</v>
+        <v>0.03187929999999949</v>
       </c>
       <c r="B17" t="n">
-        <v>0.3271829186070354</v>
+        <v>-0.2900484156769752</v>
       </c>
       <c r="C17" t="n">
-        <v>0.005380600201584886</v>
+        <v>0.01450449659839718</v>
       </c>
       <c r="D17" t="n">
-        <v>62.20673974235961</v>
+        <v>61.9403494263091</v>
       </c>
       <c r="E17" t="n">
-        <v>-79.38237905458644</v>
+        <v>-81.33530838608252</v>
       </c>
       <c r="F17" t="n">
         <v>15</v>
@@ -787,19 +787,19 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0.01277602165241459</v>
+        <v>0.02738696666666629</v>
       </c>
       <c r="B18" t="n">
-        <v>0.1632611229311623</v>
+        <v>-0.4952661885593346</v>
       </c>
       <c r="C18" t="n">
-        <v>0.006320965955682019</v>
+        <v>0.01410683746600191</v>
       </c>
       <c r="D18" t="n">
-        <v>27.15632824073893</v>
+        <v>21.88413086905823</v>
       </c>
       <c r="E18" t="n">
-        <v>-50.78388276646678</v>
+        <v>-73.64613924139852</v>
       </c>
       <c r="F18" t="n">
         <v>16</v>
@@ -807,19 +807,19 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0.009184853667081782</v>
+        <v>0.02356666666666625</v>
       </c>
       <c r="B19" t="n">
-        <v>0.1876403846026099</v>
+        <v>-0.4831209571760536</v>
       </c>
       <c r="C19" t="n">
-        <v>0.005946669553404348</v>
+        <v>0.01344244939790623</v>
       </c>
       <c r="D19" t="n">
-        <v>31.26249992272761</v>
+        <v>29.93576416041296</v>
       </c>
       <c r="E19" t="n">
-        <v>-67.37116608050415</v>
+        <v>-66.30320178915427</v>
       </c>
       <c r="F19" t="n">
         <v>17</v>
@@ -827,19 +827,19 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.002866464322252697</v>
+        <v>0.0176335428571426</v>
       </c>
       <c r="B20" t="n">
-        <v>0.2435478807864958</v>
+        <v>-0.4193371263871642</v>
       </c>
       <c r="C20" t="n">
-        <v>0.008378269355337786</v>
+        <v>0.01066363981611673</v>
       </c>
       <c r="D20" t="n">
-        <v>34.34349841099724</v>
+        <v>31.99562501018344</v>
       </c>
       <c r="E20" t="n">
-        <v>-72.29254313702833</v>
+        <v>-76.24182983192375</v>
       </c>
       <c r="F20" t="n">
         <v>18</v>
@@ -847,19 +847,19 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.002078510743094199</v>
+        <v>0.01688125520833304</v>
       </c>
       <c r="B21" t="n">
-        <v>0.1845282344935664</v>
+        <v>-0.4759898255524047</v>
       </c>
       <c r="C21" t="n">
-        <v>0.005325596082023524</v>
+        <v>0.01193641439824343</v>
       </c>
       <c r="D21" t="n">
-        <v>35.54178086282234</v>
+        <v>28.25464481318303</v>
       </c>
       <c r="E21" t="n">
-        <v>-70.26433410178562</v>
+        <v>-84.48462977081785</v>
       </c>
       <c r="F21" t="n">
         <v>19</v>
@@ -867,19 +867,19 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0.01097339483756912</v>
+        <v>0.0256956999999996</v>
       </c>
       <c r="B22" t="n">
-        <v>0.1262704788765468</v>
+        <v>-0.516632783353136</v>
       </c>
       <c r="C22" t="n">
-        <v>0.004769659520192954</v>
+        <v>0.0143637551531884</v>
       </c>
       <c r="D22" t="n">
-        <v>43.28600926053447</v>
+        <v>38.00209543046216</v>
       </c>
       <c r="E22" t="n">
-        <v>-41.65370072769352</v>
+        <v>-61.93016930583573</v>
       </c>
       <c r="F22" t="n">
         <v>20</v>
@@ -887,19 +887,19 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0.006234698565036533</v>
+        <v>0.02085103854166638</v>
       </c>
       <c r="B23" t="n">
-        <v>0.1822255452505377</v>
+        <v>-0.4791163098488145</v>
       </c>
       <c r="C23" t="n">
-        <v>0.006497059408533399</v>
+        <v>0.01254157844963881</v>
       </c>
       <c r="D23" t="n">
-        <v>27.67473969566274</v>
+        <v>21.1960434028457</v>
       </c>
       <c r="E23" t="n">
-        <v>-57.40356582818455</v>
+        <v>-72.19888026138942</v>
       </c>
       <c r="F23" t="n">
         <v>21</v>
@@ -907,19 +907,19 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0.00513491467248337</v>
+        <v>0.0198869323601969</v>
       </c>
       <c r="B24" t="n">
-        <v>0.00588135787470902</v>
+        <v>-0.6493123890965078</v>
       </c>
       <c r="C24" t="n">
-        <v>0.004168230232110934</v>
+        <v>0.01457858597115233</v>
       </c>
       <c r="D24" t="n">
-        <v>42.91778683065272</v>
+        <v>38.06348417639627</v>
       </c>
       <c r="E24" t="n">
-        <v>-40.41788011606975</v>
+        <v>-56.92832554438967</v>
       </c>
       <c r="F24" t="n">
         <v>22</v>
@@ -927,19 +927,19 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0.005376217746727448</v>
+        <v>0.0201829787709797</v>
       </c>
       <c r="B25" t="n">
-        <v>-0.02325644003000819</v>
+        <v>-0.667705284466882</v>
       </c>
       <c r="C25" t="n">
-        <v>0.003758026797506845</v>
+        <v>0.01529077329480307</v>
       </c>
       <c r="D25" t="n">
-        <v>35.20149788051975</v>
+        <v>29.37582716036991</v>
       </c>
       <c r="E25" t="n">
-        <v>-46.65545164026287</v>
+        <v>-59.75109517053831</v>
       </c>
       <c r="F25" t="n">
         <v>23</v>
@@ -947,19 +947,19 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0.00483635662983685</v>
+        <v>0.01942165245889042</v>
       </c>
       <c r="B26" t="n">
-        <v>0.05741663671836112</v>
+        <v>-0.6041265854581094</v>
       </c>
       <c r="C26" t="n">
-        <v>0.003730438096506507</v>
+        <v>0.01393560204946034</v>
       </c>
       <c r="D26" t="n">
-        <v>48.08190431054824</v>
+        <v>46.48894368597867</v>
       </c>
       <c r="E26" t="n">
-        <v>-64.59116634311304</v>
+        <v>-67.5379172464626</v>
       </c>
       <c r="F26" t="n">
         <v>24</v>
@@ -967,19 +967,19 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>0.0026746514566514</v>
+        <v>0.01717669349123039</v>
       </c>
       <c r="B27" t="n">
-        <v>0.01584425828584345</v>
+        <v>-0.650699980811523</v>
       </c>
       <c r="C27" t="n">
-        <v>0.002063345441072744</v>
+        <v>0.01486336823295297</v>
       </c>
       <c r="D27" t="n">
-        <v>39.84994971997929</v>
+        <v>33.33084147069215</v>
       </c>
       <c r="E27" t="n">
-        <v>-56.53078962697166</v>
+        <v>-68.31909724871178</v>
       </c>
       <c r="F27" t="n">
         <v>25</v>
@@ -987,19 +987,19 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>0.006714176797792768</v>
+        <v>0.02122841387036161</v>
       </c>
       <c r="B28" t="n">
-        <v>-0.03158908954096089</v>
+        <v>-0.6803653909792889</v>
       </c>
       <c r="C28" t="n">
-        <v>0.004751901111793445</v>
+        <v>0.01608332701901606</v>
       </c>
       <c r="D28" t="n">
-        <v>39.16005634655902</v>
+        <v>37.76875511559213</v>
       </c>
       <c r="E28" t="n">
-        <v>-51.99881467912345</v>
+        <v>-51.75771851419073</v>
       </c>
       <c r="F28" t="n">
         <v>26</v>
@@ -1007,19 +1007,19 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>-0.001693836225436336</v>
+        <v>0.01304621389018141</v>
       </c>
       <c r="B29" t="n">
-        <v>0.2072997783691784</v>
+        <v>-0.460428630672934</v>
       </c>
       <c r="C29" t="n">
-        <v>0.005098871097328627</v>
+        <v>0.01086760150764514</v>
       </c>
       <c r="D29" t="n">
-        <v>41.76056848758277</v>
+        <v>36.81280712484585</v>
       </c>
       <c r="E29" t="n">
-        <v>-37.99410850835997</v>
+        <v>-55.48258067246545</v>
       </c>
       <c r="F29" t="n">
         <v>27</v>
@@ -1027,19 +1027,19 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0.002330665727222756</v>
+        <v>0.0171354159736838</v>
       </c>
       <c r="B30" t="n">
-        <v>0.08029727403436233</v>
+        <v>-0.557945038109792</v>
       </c>
       <c r="C30" t="n">
-        <v>0.003238637763507987</v>
+        <v>0.01327944039906333</v>
       </c>
       <c r="D30" t="n">
-        <v>38.37018805138749</v>
+        <v>32.62328107762917</v>
       </c>
       <c r="E30" t="n">
-        <v>-50.28915177815563</v>
+        <v>-65.38925204724993</v>
       </c>
       <c r="F30" t="n">
         <v>28</v>
@@ -1047,19 +1047,19 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>0.001851609066906718</v>
+        <v>0.01669786562914701</v>
       </c>
       <c r="B31" t="n">
-        <v>0.06012627387253142</v>
+        <v>-0.5791854679963012</v>
       </c>
       <c r="C31" t="n">
-        <v>0.002653532385341967</v>
+        <v>0.01377611248523513</v>
       </c>
       <c r="D31" t="n">
-        <v>32.22939598880857</v>
+        <v>30.12708172981849</v>
       </c>
       <c r="E31" t="n">
-        <v>-66.33103358886862</v>
+        <v>-70.00280588147028</v>
       </c>
       <c r="F31" t="n">
         <v>29</v>
@@ -1067,19 +1067,19 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>0.0100494872671646</v>
+        <v>0.02460342249999979</v>
       </c>
       <c r="B32" t="n">
-        <v>-0.3598738674937444</v>
+        <v>-1.00242956574095</v>
       </c>
       <c r="C32" t="n">
-        <v>0.006856646187861419</v>
+        <v>0.02196530719355607</v>
       </c>
       <c r="D32" t="n">
-        <v>11.01814695122591</v>
+        <v>8.958492269745213</v>
       </c>
       <c r="E32" t="n">
-        <v>-9.608064070489965</v>
+        <v>-12.1072120678675</v>
       </c>
       <c r="F32" t="n">
         <v>30</v>
@@ -1087,19 +1087,19 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>0.0007339728299216452</v>
+        <v>0.01531722854212956</v>
       </c>
       <c r="B33" t="n">
-        <v>-0.04715314444366168</v>
+        <v>-0.7023149468219593</v>
       </c>
       <c r="C33" t="n">
-        <v>0.001510929242360452</v>
+        <v>0.01645038932621357</v>
       </c>
       <c r="D33" t="n">
-        <v>19.78744087512309</v>
+        <v>17.33980085159854</v>
       </c>
       <c r="E33" t="n">
-        <v>-59.21353538232588</v>
+        <v>-92.01874341558198</v>
       </c>
       <c r="F33" t="n">
         <v>31</v>
@@ -1107,19 +1107,19 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>0.00565511710181539</v>
+        <v>0.02005938349849735</v>
       </c>
       <c r="B34" t="n">
-        <v>-0.1822266930381763</v>
+        <v>-0.8371256729959542</v>
       </c>
       <c r="C34" t="n">
-        <v>0.004259163515995619</v>
+        <v>0.01795984244250424</v>
       </c>
       <c r="D34" t="n">
-        <v>20.9308915086084</v>
+        <v>19.53146198129168</v>
       </c>
       <c r="E34" t="n">
-        <v>-50.3774663521443</v>
+        <v>-86.86632210679339</v>
       </c>
       <c r="F34" t="n">
         <v>32</v>
@@ -1127,19 +1127,19 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>0.005019019614673753</v>
+        <v>0.01970191438883411</v>
       </c>
       <c r="B35" t="n">
-        <v>-0.1619196163743815</v>
+        <v>-0.7928128300649632</v>
       </c>
       <c r="C35" t="n">
-        <v>0.004201990327278174</v>
+        <v>0.01857757543702953</v>
       </c>
       <c r="D35" t="n">
-        <v>19.57587411217437</v>
+        <v>13.67992466406772</v>
       </c>
       <c r="E35" t="n">
-        <v>-49.4390421254724</v>
+        <v>-108.7760421171383</v>
       </c>
       <c r="F35" t="n">
         <v>33</v>
@@ -1147,19 +1147,19 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>0.001585721261110376</v>
+        <v>0.01616103368388381</v>
       </c>
       <c r="B36" t="n">
-        <v>-0.08420676243206225</v>
+        <v>-0.7344788531821792</v>
       </c>
       <c r="C36" t="n">
-        <v>0.001781603747779381</v>
+        <v>0.01680391572955407</v>
       </c>
       <c r="D36" t="n">
-        <v>20.80094986944983</v>
+        <v>19.44638498139446</v>
       </c>
       <c r="E36" t="n">
-        <v>-50.18766739303585</v>
+        <v>-82.5016456698483</v>
       </c>
       <c r="F36" t="n">
         <v>34</v>
@@ -1167,19 +1167,19 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>0.003638466906014801</v>
+        <v>0.01818225848422167</v>
       </c>
       <c r="B37" t="n">
-        <v>-0.1331171612016337</v>
+        <v>-0.7876842709308629</v>
       </c>
       <c r="C37" t="n">
-        <v>0.002538966893398722</v>
+        <v>0.01713919452276819</v>
       </c>
       <c r="D37" t="n">
-        <v>12.98525938162125</v>
+        <v>11.37741414608985</v>
       </c>
       <c r="E37" t="n">
-        <v>-63.76945084478938</v>
+        <v>-90.38536625301617</v>
       </c>
       <c r="F37" t="n">
         <v>35</v>
@@ -1187,19 +1187,19 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>0.004996495700326854</v>
+        <v>0.01969223741332427</v>
       </c>
       <c r="B38" t="n">
-        <v>-0.1896409366880591</v>
+        <v>-0.8308961020123464</v>
       </c>
       <c r="C38" t="n">
-        <v>0.00425573512797767</v>
+        <v>0.01939952079340379</v>
       </c>
       <c r="D38" t="n">
-        <v>16.0994107644036</v>
+        <v>13.41435035713817</v>
       </c>
       <c r="E38" t="n">
-        <v>-73.56742789005463</v>
+        <v>-101.2166942433644</v>
       </c>
       <c r="F38" t="n">
         <v>36</v>
@@ -1207,19 +1207,19 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>0.007419953615086644</v>
+        <v>0.02196707833790037</v>
       </c>
       <c r="B39" t="n">
-        <v>-0.1921566973228025</v>
+        <v>-0.8473047673472127</v>
       </c>
       <c r="C39" t="n">
-        <v>0.004808294806688117</v>
+        <v>0.01817307655378765</v>
       </c>
       <c r="D39" t="n">
-        <v>18.08096162301872</v>
+        <v>16.28047606733938</v>
       </c>
       <c r="E39" t="n">
-        <v>-46.98239848817071</v>
+        <v>-82.83675410526831</v>
       </c>
       <c r="F39" t="n">
         <v>37</v>
@@ -1227,19 +1227,19 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>0.01100494228349626</v>
+        <v>0.02534582564787492</v>
       </c>
       <c r="B40" t="n">
-        <v>-0.4391384069867468</v>
+        <v>-1.087081346340354</v>
       </c>
       <c r="C40" t="n">
-        <v>0.007817119392250431</v>
+        <v>0.0242421500529274</v>
       </c>
       <c r="D40" t="n">
-        <v>12.56635015022701</v>
+        <v>13.65391634351252</v>
       </c>
       <c r="E40" t="n">
-        <v>-9.350520304598183</v>
+        <v>-7.120863890885293</v>
       </c>
       <c r="F40" t="n">
         <v>38</v>
@@ -1247,19 +1247,19 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>-0.001403690472340024</v>
+        <v>0.01331892569291484</v>
       </c>
       <c r="B41" t="n">
-        <v>0.1212159762492618</v>
+        <v>-0.5294083889143651</v>
       </c>
       <c r="C41" t="n">
-        <v>0.002633551022753115</v>
+        <v>0.01218165047656733</v>
       </c>
       <c r="D41" t="n">
-        <v>19.24442053694606</v>
+        <v>18.04556296199106</v>
       </c>
       <c r="E41" t="n">
-        <v>-49.12251450380327</v>
+        <v>-72.9745672578326</v>
       </c>
       <c r="F41" t="n">
         <v>39</v>
@@ -1267,19 +1267,19 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>0.003998759063008198</v>
+        <v>0.01866133842757729</v>
       </c>
       <c r="B42" t="n">
-        <v>-0.07155415964064167</v>
+        <v>-0.7226529194067505</v>
       </c>
       <c r="C42" t="n">
-        <v>0.003232474042622202</v>
+        <v>0.01705057858899307</v>
       </c>
       <c r="D42" t="n">
-        <v>19.59803963002415</v>
+        <v>18.010380305741</v>
       </c>
       <c r="E42" t="n">
-        <v>-52.0593832450757</v>
+        <v>-88.34238076227761</v>
       </c>
       <c r="F42" t="n">
         <v>40</v>

</xml_diff>